<commit_message>
fetcher finished + files added
</commit_message>
<xml_diff>
--- a/data-fetching/werkzittingen/template_wz1.xlsx
+++ b/data-fetching/werkzittingen/template_wz1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff\Documents\Kuleuven\FeedbackVisuals\FeedbackVisuals\data-fetching\werkzittingen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33623BDF-8B23-494B-8944-7A615E270873}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35AA064-FB3F-4C88-B6CC-200E7D7DAC35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ECCF5C31-E73D-41E6-A20B-1B020134CB8E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Q4</t>
   </si>
@@ -72,18 +72,58 @@
     <t>maximale score</t>
   </si>
   <si>
-    <t>WZ1 
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WZ1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 Questions</t>
+    </r>
+  </si>
+  <si>
+    <t>gewicht vraag</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -115,11 +155,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -435,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA8FD038-3A68-48E2-8948-48864369A52F}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,9 +502,10 @@
     <col min="2" max="2" width="39.5546875" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -460,332 +516,376 @@
         <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1">
+      <c r="F1" s="3">
+        <v>1</v>
+      </c>
+      <c r="G1" s="3">
         <v>2</v>
       </c>
-      <c r="G1" s="1">
+      <c r="H1" s="3">
         <v>3</v>
       </c>
-      <c r="H1" s="1">
+      <c r="I1" s="3">
         <v>4</v>
       </c>
-      <c r="I1" s="1">
+      <c r="J1" s="3">
         <v>5</v>
       </c>
-      <c r="J1" s="1">
+      <c r="K1" s="3">
         <v>6</v>
       </c>
-      <c r="K1" s="1">
+      <c r="L1" s="3">
         <v>7</v>
       </c>
-      <c r="L1" s="1">
+      <c r="M1" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="6">
         <v>0.5</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="J2" s="5">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="E3" s="7">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="4">
         <v>0.5</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="K4" s="4">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
         <v>0.5</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>2</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
         <v>0.5</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>3</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>3</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>4</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="7">
         <v>4.5</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4">
+        <v>1</v>
+      </c>
+      <c r="I10" s="4">
+        <v>1</v>
+      </c>
+      <c r="J10" s="4">
+        <v>1</v>
+      </c>
+      <c r="K10" s="4">
         <v>0.5</v>
       </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>